<commit_message>
Update Switching Losses and Output Control
</commit_message>
<xml_diff>
--- a/para/templateCap.xlsx
+++ b/para/templateCap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="367" documentId="11_AD4DB114E441178AC67DF439BED5CE16693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D5EDEC4-8C43-4DA1-8791-54855B263C70}"/>
   <bookViews>
-    <workbookView xWindow="4356" yWindow="2220" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -10891,6 +10891,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11156,7 +11160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
@@ -11266,7 +11270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8064A7B3-208D-49B4-A622-7BE04E7FA670}">
   <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B93" sqref="B93:C96"/>
     </sheetView>
   </sheetViews>
@@ -12798,7 +12802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB07583-2F94-4C44-B797-F29E5519DCF0}">
   <dimension ref="A1:P148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>

</xml_diff>